<commit_message>
setup where most effectors randomly generated
</commit_message>
<xml_diff>
--- a/effector_inputs_RAND.xlsx
+++ b/effector_inputs_RAND.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmontunnas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0C33161-EC41-A141-A074-37016E87721F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910CDFC4-FCB8-1F48-B491-7C733A3052FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{B8EEBF2D-FDDC-2849-BD58-E0F5226AEB01}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,6 +447,15 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Mostly random effector setup
</commit_message>
<xml_diff>
--- a/effector_inputs_RAND.xlsx
+++ b/effector_inputs_RAND.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmontunnas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910CDFC4-FCB8-1F48-B491-7C733A3052FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A029F9-5F9C-9345-BF97-DDC75FF9EBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{B8EEBF2D-FDDC-2849-BD58-E0F5226AEB01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t>Effector X (m)</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Effector Type (0 = Fixed)</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,6 +449,62 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>

</xml_diff>